<commit_message>
remove all hard-coded data from STRATEGIC model
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_strategic_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_strategic_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00073B64-3097-46FC-ABB3-EC063E8F00FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D67D4D-9554-4409-B02E-763E60FF1E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="31" activeTab="36" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="36" activeTab="37" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -47,11 +47,10 @@
     <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId32"/>
     <sheet name="TruckingTime" sheetId="7" r:id="rId33"/>
     <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId34"/>
-    <sheet name="TreatmentlOperationalCost" sheetId="68" r:id="rId35"/>
+    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId35"/>
     <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId36"/>
     <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId37"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId38"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId39"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId38"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -63,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="123">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -74,21 +73,12 @@
     <t>List of all SWD Sites [-]</t>
   </si>
   <si>
-    <t>PP01</t>
-  </si>
-  <si>
     <t>PP02</t>
   </si>
   <si>
     <t>PP03</t>
   </si>
   <si>
-    <t>PP04</t>
-  </si>
-  <si>
-    <t>PP05</t>
-  </si>
-  <si>
     <t>CP01</t>
   </si>
   <si>
@@ -330,9 +320,6 @@
   </si>
   <si>
     <t>Table of Reuse Operational Cost  [$/bbl]</t>
-  </si>
-  <si>
-    <t>Table of Trucking Hourly Cost  [$/hour]</t>
   </si>
   <si>
     <t>Table of Freshwater Sourcing Cost  [$/hour]</t>
@@ -1159,7 +1146,7 @@
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="18"/>
       <c r="C3" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
@@ -1185,7 +1172,7 @@
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="18"/>
       <c r="C5" s="20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -1199,7 +1186,7 @@
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="18"/>
       <c r="C6" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -1213,7 +1200,7 @@
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="18"/>
       <c r="C7" s="20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -1227,7 +1214,7 @@
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="C8" s="20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
@@ -1241,7 +1228,7 @@
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="C9" s="20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
@@ -1255,7 +1242,7 @@
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -1281,7 +1268,7 @@
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
@@ -1295,7 +1282,7 @@
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
@@ -1321,7 +1308,7 @@
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
       <c r="C15" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
@@ -1335,7 +1322,7 @@
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="18"/>
       <c r="C16" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
@@ -1349,7 +1336,7 @@
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
       <c r="C17" s="20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
@@ -1363,7 +1350,7 @@
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
       <c r="C18" s="20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
@@ -1401,12 +1388,12 @@
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>
       <c r="C21" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
@@ -1429,12 +1416,12 @@
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="18"/>
       <c r="C23" s="23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -1445,12 +1432,12 @@
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="18"/>
       <c r="C24" s="23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -1461,12 +1448,12 @@
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="18"/>
       <c r="C25" s="23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -1477,12 +1464,12 @@
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="18"/>
       <c r="C26" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -1493,12 +1480,12 @@
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="18"/>
       <c r="C27" s="23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -1509,12 +1496,12 @@
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="18"/>
       <c r="C28" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -1525,12 +1512,12 @@
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="18"/>
       <c r="C29" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
@@ -1541,12 +1528,12 @@
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
       <c r="C30" s="23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
@@ -1557,12 +1544,12 @@
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
       <c r="C31" s="23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
@@ -1570,18 +1557,18 @@
       <c r="J31" s="20"/>
       <c r="K31" s="21"/>
       <c r="M31" s="27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
       <c r="C32" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -1592,12 +1579,12 @@
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="18"/>
       <c r="C33" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
@@ -1608,12 +1595,12 @@
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="18"/>
       <c r="C34" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
@@ -1624,12 +1611,12 @@
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="18"/>
       <c r="C35" s="23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
@@ -1640,12 +1627,12 @@
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="18"/>
       <c r="C36" s="23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
@@ -1710,17 +1697,17 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1743,7 +1730,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1766,7 +1753,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1789,7 +1776,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1812,7 +1799,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1835,7 +1822,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1906,17 +1893,17 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1939,7 +1926,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1962,7 +1949,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1985,7 +1972,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2008,7 +1995,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2078,12 +2065,12 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2240,12 +2227,12 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2394,21 +2381,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
@@ -2417,7 +2404,7 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="12">
@@ -2445,18 +2432,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="28" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
@@ -2483,36 +2470,36 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="H2" s="28" t="s">
         <v>95</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10">
@@ -2528,7 +2515,7 @@
     </row>
     <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -2544,7 +2531,7 @@
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10">
@@ -2560,7 +2547,7 @@
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B6" s="10">
         <v>1</v>
@@ -2576,7 +2563,7 @@
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -2592,7 +2579,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2608,7 +2595,7 @@
     </row>
     <row r="9" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -2644,18 +2631,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
@@ -2682,18 +2669,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
@@ -2720,18 +2707,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="28" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
@@ -2770,7 +2757,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2791,7 +2778,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="13"/>
@@ -2832,18 +2819,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" s="33">
         <v>1</v>
@@ -2851,7 +2838,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
@@ -2868,7 +2855,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2878,18 +2865,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
@@ -2916,18 +2903,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="33">
         <v>1</v>
@@ -2935,7 +2922,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
@@ -2963,7 +2950,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3017,7 +3004,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3049,18 +3036,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
@@ -3077,7 +3064,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3087,30 +3074,30 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="F2" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="11">
         <v>315000</v>
@@ -3194,30 +3181,30 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="F2" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="10">
         <v>14000</v>
@@ -3237,7 +3224,7 @@
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="11">
         <v>8000</v>
@@ -3321,45 +3308,45 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="28" t="s">
         <v>92</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -3376,7 +3363,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B4" s="10">
         <v>210000</v>
@@ -3395,7 +3382,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10">
@@ -3416,7 +3403,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B6" s="10">
         <v>20000</v>
@@ -3433,7 +3420,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B7" s="10">
         <v>210000</v>
@@ -3452,7 +3439,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -3471,7 +3458,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -3488,7 +3475,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -3505,7 +3492,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -3526,7 +3513,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -3547,7 +3534,7 @@
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -3665,7 +3652,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3674,7 +3661,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" s="12">
         <v>210000</v>
@@ -3708,12 +3695,12 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -3734,7 +3721,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3755,7 +3742,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="13"/>
@@ -3776,7 +3763,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -3797,7 +3784,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3818,47 +3805,47 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3883,7 +3870,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3892,7 +3879,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B3" s="12">
         <v>50000</v>
@@ -3919,30 +3906,30 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="F2" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" s="10">
         <v>180000</v>
@@ -3962,7 +3949,7 @@
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="11">
         <v>160000</v>
@@ -4046,7 +4033,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4055,7 +4042,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="12">
         <v>210000</v>
@@ -4082,18 +4069,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="33">
         <v>3</v>
@@ -4101,7 +4088,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="12">
         <v>4</v>
@@ -4158,7 +4145,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4167,7 +4154,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" s="12">
         <v>0.4</v>
@@ -4184,7 +4171,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4194,7 +4181,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4203,7 +4190,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
@@ -4220,7 +4207,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4230,7 +4217,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4239,7 +4226,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="12">
         <v>0.7</v>
@@ -4255,7 +4242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE24AD9-42B2-417F-BF2D-D0F067DA599C}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4266,24 +4253,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
@@ -4293,7 +4280,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10">
@@ -4303,7 +4290,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -4313,7 +4300,7 @@
     </row>
     <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -4328,11 +4315,11 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4342,7 +4329,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4351,83 +4338,7 @@
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="33">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="33">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="33">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="33">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="33">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="12">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" s="33">
         <v>0.1</v>
@@ -4435,7 +4346,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="12">
         <v>0.12</v>
@@ -4475,7 +4386,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -4651,7 +4562,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -4772,17 +4683,17 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4953,12 +4864,12 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -5131,12 +5042,12 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -5309,7 +5220,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completions storage strategic model
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_strategic_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_strategic_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A275B4DC-5C39-472B-B79B-EDA1AC5FC040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8DCA56-499A-438B-BCE9-158E1A0BA3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="32" activeTab="33" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="32" activeTab="32" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -45,14 +45,15 @@
     <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId30"/>
     <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId31"/>
     <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId32"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId33"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId34"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId35"/>
-    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId36"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId37"/>
-    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId38"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId39"/>
-    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId40"/>
+    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId33"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId34"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId35"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId36"/>
+    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId37"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId38"/>
+    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId39"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId40"/>
+    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId41"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="126">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -439,6 +440,9 @@
   </si>
   <si>
     <t>Table of Trucking Hourly Cost  [$/hour]</t>
+  </si>
+  <si>
+    <t>Table of Completoins Pad Storage Capacity  [bbl]</t>
   </si>
 </sst>
 </file>
@@ -4073,6 +4077,42 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB793D-71C1-4CA2-A5D0-D94D2FB81D42}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12">
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4108,11 +4148,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4200,7 +4240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4236,7 +4276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7050C77-5C7B-4C97-8F2B-C60EA6AF1AED}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4272,7 +4312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4308,7 +4348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE24AD9-42B2-417F-BF2D-D0F067DA599C}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -4376,50 +4416,6 @@
       <c r="C6" s="11"/>
       <c r="D6" s="12">
         <v>0.3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="33">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0.12</v>
       </c>
     </row>
   </sheetData>
@@ -4607,6 +4603,50 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35585569-7889-4883-A327-3B12D4AB6358}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
improved flowback processing - strategic
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_strategic_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_strategic_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8DCA56-499A-438B-BCE9-158E1A0BA3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944339E3-83EF-4B65-9A40-08BCFB4504A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="32" activeTab="32" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="390" yWindow="300" windowWidth="37200" windowHeight="20700" activeTab="16" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -28,32 +28,35 @@
     <sheet name="InjectionCapacities" sheetId="55" r:id="rId13"/>
     <sheet name="PNA" sheetId="56" r:id="rId14"/>
     <sheet name="CNA" sheetId="57" r:id="rId15"/>
-    <sheet name="NNA" sheetId="58" r:id="rId16"/>
-    <sheet name="NCA" sheetId="59" r:id="rId17"/>
-    <sheet name="NKA" sheetId="60" r:id="rId18"/>
-    <sheet name="NRA" sheetId="61" r:id="rId19"/>
-    <sheet name="FCA" sheetId="41" r:id="rId20"/>
-    <sheet name="RNA" sheetId="62" r:id="rId21"/>
-    <sheet name="PCT" sheetId="42" r:id="rId22"/>
-    <sheet name="FCT" sheetId="70" r:id="rId23"/>
-    <sheet name="PKT" sheetId="43" r:id="rId24"/>
-    <sheet name="CKT" sheetId="44" r:id="rId25"/>
-    <sheet name="CST" sheetId="64" r:id="rId26"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId27"/>
-    <sheet name="PadRates" sheetId="65" r:id="rId28"/>
-    <sheet name="InitialPipelineCapacity" sheetId="66" r:id="rId29"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId30"/>
-    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId31"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId32"/>
-    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId33"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId34"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId35"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId36"/>
-    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId37"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId38"/>
-    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId39"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId40"/>
-    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId41"/>
+    <sheet name="CCA" sheetId="73" r:id="rId16"/>
+    <sheet name="NNA" sheetId="58" r:id="rId17"/>
+    <sheet name="NCA" sheetId="59" r:id="rId18"/>
+    <sheet name="NKA" sheetId="60" r:id="rId19"/>
+    <sheet name="NRA" sheetId="61" r:id="rId20"/>
+    <sheet name="FCA" sheetId="41" r:id="rId21"/>
+    <sheet name="RNA" sheetId="62" r:id="rId22"/>
+    <sheet name="PCT" sheetId="42" r:id="rId23"/>
+    <sheet name="FCT" sheetId="70" r:id="rId24"/>
+    <sheet name="PKT" sheetId="43" r:id="rId25"/>
+    <sheet name="CKT" sheetId="44" r:id="rId26"/>
+    <sheet name="CCT" sheetId="74" r:id="rId27"/>
+    <sheet name="CST" sheetId="64" r:id="rId28"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId29"/>
+    <sheet name="PadRates" sheetId="65" r:id="rId30"/>
+    <sheet name="FlowbackRates" sheetId="75" r:id="rId31"/>
+    <sheet name="InitialPipelineCapacity" sheetId="66" r:id="rId32"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId33"/>
+    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId34"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId35"/>
+    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId36"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId37"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId38"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId39"/>
+    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId40"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId41"/>
+    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId42"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId43"/>
+    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId44"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -65,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -443,6 +446,15 @@
   </si>
   <si>
     <t>Table of Completoins Pad Storage Capacity  [bbl]</t>
+  </si>
+  <si>
+    <t>Completions Pads to Completions Pads Piping Arcs [-]</t>
+  </si>
+  <si>
+    <t>Completions Pads to Completions Pads Trucking Arcs [-]</t>
+  </si>
+  <si>
+    <t>Table of Flowback Rate Forecasts by Pads [bbl/week]</t>
   </si>
 </sst>
 </file>
@@ -2468,10 +2480,48 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F10C60C-760C-4F1B-AB9A-B14851122200}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7399EB22-0DA7-4F9B-9913-FB50F464ABD0}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -2628,7 +2678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037676BC-0D9E-4EC2-B7DF-9077076036FD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2666,7 +2716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B147A77C-3EC6-43F3-933A-7BFD421AB782}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2693,44 +2743,6 @@
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928AC5F8-3DBD-4182-95AF-F72C7FA4D2FF}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
@@ -2817,6 +2829,44 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928AC5F8-3DBD-4182-95AF-F72C7FA4D2FF}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2862,7 +2912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3F673B-ABE6-40C2-BA6B-F7AEA69D03F8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2900,7 +2950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2947,7 +2997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F615298C-1D1C-4004-91BA-05C3C07D8B7C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2993,7 +3043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3047,7 +3097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3079,7 +3129,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37622F2B-1E4B-46C9-B210-3150CCBB5892}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A52059-0CB1-474F-ACFF-2997470BE1E9}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3117,7 +3203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -3218,478 +3304,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF4E1D-6CE0-4F02-8B9E-F2818C0A814C}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.28515625" style="9"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="10">
-        <v>14000</v>
-      </c>
-      <c r="C3" s="10">
-        <v>13800</v>
-      </c>
-      <c r="D3" s="10">
-        <v>13750</v>
-      </c>
-      <c r="E3" s="10">
-        <v>13700</v>
-      </c>
-      <c r="F3" s="33">
-        <v>13650</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="11">
-        <v>8000</v>
-      </c>
-      <c r="C4" s="11">
-        <v>7950</v>
-      </c>
-      <c r="D4" s="11">
-        <v>7900</v>
-      </c>
-      <c r="E4" s="11">
-        <v>7850</v>
-      </c>
-      <c r="F4" s="12">
-        <v>7800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE628BF-A05C-42C8-8EC7-63FF3B624ADC}">
-  <dimension ref="A1:K24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="33">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="10">
-        <v>210000</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10">
-        <v>140000</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="33"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10">
-        <v>210000</v>
-      </c>
-      <c r="D5" s="10">
-        <v>210000</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="33">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="10">
-        <v>20000</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="33"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="10">
-        <v>210000</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10">
-        <v>210000</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="33"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10">
-        <v>210000</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10">
-        <v>210000</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="33"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10">
-        <v>20000</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="33"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10">
-        <v>400000</v>
-      </c>
-      <c r="K10" s="33"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10">
-        <v>140000</v>
-      </c>
-      <c r="G11" s="10">
-        <v>210000</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10">
-        <v>400000</v>
-      </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="33"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10">
-        <v>210000</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10">
-        <v>210000</v>
-      </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10">
-        <v>210000</v>
-      </c>
-      <c r="K12" s="33"/>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11">
-        <v>140000</v>
-      </c>
-      <c r="K13" s="12">
-        <v>140000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3878,6 +3492,586 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF4E1D-6CE0-4F02-8B9E-F2818C0A814C}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" style="9"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>14000</v>
+      </c>
+      <c r="C3" s="10">
+        <v>13800</v>
+      </c>
+      <c r="D3" s="10">
+        <v>13750</v>
+      </c>
+      <c r="E3" s="10">
+        <v>13700</v>
+      </c>
+      <c r="F3" s="33">
+        <v>13650</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>8000</v>
+      </c>
+      <c r="C4" s="11">
+        <v>7950</v>
+      </c>
+      <c r="D4" s="11">
+        <v>7900</v>
+      </c>
+      <c r="E4" s="11">
+        <v>7850</v>
+      </c>
+      <c r="F4" s="12">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68666333-AE69-4574-92B2-6BE3A00DF612}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" style="9"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2500</v>
+      </c>
+      <c r="C3" s="11">
+        <v>2500</v>
+      </c>
+      <c r="D3" s="11">
+        <v>2500</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2500</v>
+      </c>
+      <c r="F3" s="12">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE628BF-A05C-42C8-8EC7-63FF3B624ADC}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="33">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="10">
+        <v>210000</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10">
+        <v>140000</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="33"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10">
+        <v>210000</v>
+      </c>
+      <c r="D5" s="10">
+        <v>210000</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="33">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="10">
+        <v>20000</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="33"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="10">
+        <v>210000</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10">
+        <v>210000</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="33"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10">
+        <v>210000</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
+        <v>210000</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="33"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10">
+        <v>20000</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="33"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10">
+        <v>400000</v>
+      </c>
+      <c r="K10" s="33"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10">
+        <v>140000</v>
+      </c>
+      <c r="G11" s="10">
+        <v>210000</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10">
+        <v>400000</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="33"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10">
+        <v>210000</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10">
+        <v>210000</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10">
+        <v>210000</v>
+      </c>
+      <c r="K12" s="33"/>
+    </row>
+    <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11">
+        <v>140000</v>
+      </c>
+      <c r="K13" s="12">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3913,7 +4107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A13F53-E3AE-452E-A1A1-316A2C800322}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3949,7 +4143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -4076,11 +4270,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB793D-71C1-4CA2-A5D0-D94D2FB81D42}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -4112,7 +4306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4148,7 +4342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -4240,7 +4434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4268,154 +4462,6 @@
       </c>
       <c r="B3" s="12">
         <v>0.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7050C77-5C7B-4C97-8F2B-C60EA6AF1AED}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="12">
-        <v>0.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE24AD9-42B2-417F-BF2D-D0F067DA599C}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="10">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="33"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="D4" s="33"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="33">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12">
-        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -4603,6 +4649,166 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7050C77-5C7B-4C97-8F2B-C60EA6AF1AED}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE24AD9-42B2-417F-BF2D-D0F067DA599C}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="33">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="33">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -4646,7 +4852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35585569-7889-4883-A327-3B12D4AB6358}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
updating get_data() and generate_report() to work with proprietary data
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_strategic_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_strategic_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944339E3-83EF-4B65-9A40-08BCFB4504A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A663E93-6432-428E-B0D6-D6DC23A8CC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="300" windowWidth="37200" windowHeight="20700" activeTab="16" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="758" firstSheet="37" activeTab="43" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="137">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -455,6 +455,30 @@
   </si>
   <si>
     <t>Table of Flowback Rate Forecasts by Pads [bbl/week]</t>
+  </si>
+  <si>
+    <t>ProductionPads</t>
+  </si>
+  <si>
+    <t>INDEX</t>
+  </si>
+  <si>
+    <t>CompletionsPads</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>SWDSites</t>
+  </si>
+  <si>
+    <t>FreshwaterSources</t>
+  </si>
+  <si>
+    <t>TreatmentSites</t>
+  </si>
+  <si>
+    <t>NetworkNodes</t>
   </si>
 </sst>
 </file>
@@ -1147,15 +1171,15 @@
       <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="4.28515625" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.26171875" customWidth="1"/>
+    <col min="10" max="10" width="4.41796875" customWidth="1"/>
+    <col min="11" max="11" width="9.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -1167,7 +1191,7 @@
       <c r="J2" s="16"/>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="18"/>
       <c r="C3" s="19" t="s">
         <v>7</v>
@@ -1181,7 +1205,7 @@
       <c r="J3" s="20"/>
       <c r="K3" s="21"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="18"/>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -1193,7 +1217,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="21"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="18"/>
       <c r="C5" s="20" t="s">
         <v>13</v>
@@ -1207,7 +1231,7 @@
       <c r="J5" s="20"/>
       <c r="K5" s="21"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="18"/>
       <c r="C6" s="20" t="s">
         <v>11</v>
@@ -1221,7 +1245,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="21"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="18"/>
       <c r="C7" s="20" t="s">
         <v>8</v>
@@ -1235,7 +1259,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="18"/>
       <c r="C8" s="20" t="s">
         <v>9</v>
@@ -1249,7 +1273,7 @@
       <c r="J8" s="20"/>
       <c r="K8" s="21"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="18"/>
       <c r="C9" s="20" t="s">
         <v>10</v>
@@ -1263,7 +1287,7 @@
       <c r="J9" s="20"/>
       <c r="K9" s="21"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="18"/>
       <c r="C10" s="20" t="s">
         <v>49</v>
@@ -1277,7 +1301,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="21"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="18"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -1289,7 +1313,7 @@
       <c r="J11" s="20"/>
       <c r="K11" s="21"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="18"/>
       <c r="C12" s="20" t="s">
         <v>14</v>
@@ -1303,7 +1327,7 @@
       <c r="J12" s="20"/>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="18"/>
       <c r="C13" s="20" t="s">
         <v>12</v>
@@ -1317,7 +1341,7 @@
       <c r="J13" s="20"/>
       <c r="K13" s="21"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="18"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -1329,7 +1353,7 @@
       <c r="J14" s="20"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="18"/>
       <c r="C15" s="20" t="s">
         <v>15</v>
@@ -1343,7 +1367,7 @@
       <c r="J15" s="20"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="18"/>
       <c r="C16" s="20" t="s">
         <v>16</v>
@@ -1357,7 +1381,7 @@
       <c r="J16" s="20"/>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="18"/>
       <c r="C17" s="20" t="s">
         <v>17</v>
@@ -1371,7 +1395,7 @@
       <c r="J17" s="20"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="18"/>
       <c r="C18" s="20" t="s">
         <v>18</v>
@@ -1385,7 +1409,7 @@
       <c r="J18" s="20"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="18"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -1397,7 +1421,7 @@
       <c r="J19" s="20"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="18"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
@@ -1409,7 +1433,7 @@
       <c r="J20" s="20"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="18"/>
       <c r="C21" s="22" t="s">
         <v>19</v>
@@ -1425,7 +1449,7 @@
       <c r="J21" s="20"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="18"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
@@ -1437,7 +1461,7 @@
       <c r="J22" s="20"/>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="18"/>
       <c r="C23" s="23" t="s">
         <v>21</v>
@@ -1453,7 +1477,7 @@
       <c r="J23" s="20"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="18"/>
       <c r="C24" s="23" t="s">
         <v>22</v>
@@ -1469,7 +1493,7 @@
       <c r="J24" s="20"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="18"/>
       <c r="C25" s="23" t="s">
         <v>23</v>
@@ -1485,7 +1509,7 @@
       <c r="J25" s="20"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="18"/>
       <c r="C26" s="23" t="s">
         <v>27</v>
@@ -1501,7 +1525,7 @@
       <c r="J26" s="20"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="18"/>
       <c r="C27" s="23" t="s">
         <v>29</v>
@@ -1517,7 +1541,7 @@
       <c r="J27" s="20"/>
       <c r="K27" s="21"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="18"/>
       <c r="C28" s="23" t="s">
         <v>31</v>
@@ -1533,7 +1557,7 @@
       <c r="J28" s="20"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="18"/>
       <c r="C29" s="23" t="s">
         <v>32</v>
@@ -1549,7 +1573,7 @@
       <c r="J29" s="20"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="18"/>
       <c r="C30" s="23" t="s">
         <v>35</v>
@@ -1565,7 +1589,7 @@
       <c r="J30" s="20"/>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="18"/>
       <c r="C31" s="23" t="s">
         <v>37</v>
@@ -1584,7 +1608,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="18"/>
       <c r="C32" s="23" t="s">
         <v>40</v>
@@ -1600,7 +1624,7 @@
       <c r="J32" s="20"/>
       <c r="K32" s="21"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="18"/>
       <c r="C33" s="23" t="s">
         <v>39</v>
@@ -1616,7 +1640,7 @@
       <c r="J33" s="20"/>
       <c r="K33" s="21"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="18"/>
       <c r="C34" s="23" t="s">
         <v>43</v>
@@ -1632,7 +1656,7 @@
       <c r="J34" s="20"/>
       <c r="K34" s="21"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="18"/>
       <c r="C35" s="23" t="s">
         <v>45</v>
@@ -1648,7 +1672,7 @@
       <c r="J35" s="20"/>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="18"/>
       <c r="C36" s="23" t="s">
         <v>46</v>
@@ -1664,7 +1688,7 @@
       <c r="J36" s="20"/>
       <c r="K36" s="21"/>
     </row>
-    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B37" s="24"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
@@ -1703,33 +1727,33 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>90</v>
       </c>
@@ -1752,7 +1776,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>91</v>
       </c>
@@ -1775,7 +1799,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>92</v>
       </c>
@@ -1798,7 +1822,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>93</v>
       </c>
@@ -1821,7 +1845,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>94</v>
       </c>
@@ -1844,7 +1868,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>95</v>
       </c>
@@ -1867,7 +1891,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1899,33 +1923,33 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>97</v>
       </c>
@@ -1948,7 +1972,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>98</v>
       </c>
@@ -1971,7 +1995,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>99</v>
       </c>
@@ -1994,7 +2018,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>100</v>
       </c>
@@ -2017,7 +2041,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>101</v>
       </c>
@@ -2040,7 +2064,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2074,30 +2098,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2118,7 +2142,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2139,7 +2163,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -2160,7 +2184,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2181,7 +2205,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2202,7 +2226,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2236,30 +2260,30 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2280,7 +2304,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2301,7 +2325,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -2322,7 +2346,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2343,7 +2367,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2364,7 +2388,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2395,21 +2419,23 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>92</v>
       </c>
@@ -2417,7 +2443,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2426,7 +2452,7 @@
       </c>
       <c r="C3" s="33"/>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2446,26 +2472,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -2484,26 +2512,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -2521,22 +2551,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7399EB22-0DA7-4F9B-9913-FB50F464ABD0}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>89</v>
       </c>
@@ -2559,7 +2591,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="29" t="s">
         <v>89</v>
       </c>
@@ -2575,7 +2607,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="33"/>
     </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="29" t="s">
         <v>90</v>
       </c>
@@ -2591,7 +2623,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="33"/>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="29" t="s">
         <v>91</v>
       </c>
@@ -2607,7 +2639,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="33"/>
     </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="29" t="s">
         <v>92</v>
       </c>
@@ -2623,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="29" t="s">
         <v>93</v>
       </c>
@@ -2639,7 +2671,7 @@
       </c>
       <c r="H7" s="33"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="29" t="s">
         <v>94</v>
       </c>
@@ -2655,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="31" t="s">
         <v>95</v>
       </c>
@@ -2683,26 +2715,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>90</v>
       </c>
@@ -2721,26 +2755,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>91</v>
       </c>
@@ -2759,27 +2795,27 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="9.28515625" style="1"/>
-    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.28515625" style="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="2" width="9.26171875" style="1"/>
+    <col min="3" max="3" width="3.578125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.26171875" style="1"/>
+    <col min="13" max="13" width="11.26171875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.83984375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.578125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -2800,7 +2836,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -2833,26 +2869,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>95</v>
       </c>
@@ -2871,26 +2909,28 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>72</v>
       </c>
@@ -2898,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="4" t="s">
         <v>73</v>
       </c>
@@ -2917,26 +2957,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>135</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
@@ -2955,26 +2997,28 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -2982,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="31" t="s">
         <v>4</v>
       </c>
@@ -3002,26 +3046,28 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>72</v>
       </c>
@@ -3029,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="4" t="s">
         <v>73</v>
       </c>
@@ -3051,42 +3097,42 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="28"/>
     </row>
-    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="29"/>
       <c r="B3" s="10"/>
       <c r="C3" s="33"/>
     </row>
-    <row r="4" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="29"/>
       <c r="B4" s="10"/>
       <c r="C4" s="33"/>
     </row>
-    <row r="5" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="29"/>
       <c r="B5" s="34"/>
       <c r="C5" s="33"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="29"/>
       <c r="B6" s="34"/>
       <c r="C6" s="33"/>
     </row>
-    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="31"/>
       <c r="B7" s="35"/>
       <c r="C7" s="12"/>
@@ -3105,21 +3151,21 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7"/>
       <c r="B2" s="28"/>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="9" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31"/>
       <c r="B3" s="12"/>
     </row>
@@ -3137,23 +3183,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="9" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
@@ -3170,26 +3218,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="9" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
@@ -3208,21 +3258,23 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>53</v>
       </c>
@@ -3239,7 +3291,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -3257,47 +3309,47 @@
       </c>
       <c r="F3" s="12"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -3317,24 +3369,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="9.28515625" style="1"/>
-    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.28515625" style="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="2" width="9.26171875" style="1"/>
+    <col min="3" max="3" width="3.578125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.26171875" style="1"/>
+    <col min="13" max="13" width="11.26171875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.83984375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.578125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>58</v>
       </c>
@@ -3355,7 +3407,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
@@ -3376,7 +3428,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>60</v>
       </c>
@@ -3397,7 +3449,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
@@ -3418,7 +3470,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
@@ -3439,47 +3491,47 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5" t="s">
         <v>71</v>
       </c>
@@ -3499,19 +3551,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="9"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="9.26171875" style="9"/>
+    <col min="2" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="32" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>53</v>
       </c>
@@ -3528,7 +3582,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
@@ -3548,7 +3602,7 @@
         <v>13650</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="31" t="s">
         <v>4</v>
       </c>
@@ -3568,47 +3622,47 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -3624,22 +3678,24 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="9"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="9.26171875" style="9"/>
+    <col min="2" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="32" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>53</v>
       </c>
@@ -3656,7 +3712,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
@@ -3676,47 +3732,47 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -3732,21 +3788,23 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>95</v>
       </c>
@@ -3778,7 +3836,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -3795,7 +3853,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>92</v>
       </c>
@@ -3814,7 +3872,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="33"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>95</v>
       </c>
@@ -3835,7 +3893,7 @@
         <v>210000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>88</v>
       </c>
@@ -3852,7 +3910,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="33"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>94</v>
       </c>
@@ -3871,7 +3929,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="33"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>93</v>
       </c>
@@ -3890,7 +3948,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="33"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -3907,7 +3965,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="33"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -3924,7 +3982,7 @@
       </c>
       <c r="K10" s="33"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>90</v>
       </c>
@@ -3945,7 +4003,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="33"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>91</v>
       </c>
@@ -3966,7 +4024,7 @@
       </c>
       <c r="K12" s="33"/>
     </row>
-    <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A13" s="4" t="s">
         <v>89</v>
       </c>
@@ -3985,7 +4043,7 @@
         <v>140000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -3993,7 +4051,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -4001,7 +4059,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -4009,7 +4067,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="14"/>
@@ -4017,7 +4075,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -4025,7 +4083,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -4033,7 +4091,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -4041,7 +4099,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -4049,7 +4107,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -4057,7 +4115,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -4076,24 +4134,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>51</v>
       </c>
@@ -4115,21 +4177,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>88</v>
       </c>
@@ -4148,21 +4214,23 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>53</v>
       </c>
@@ -4179,7 +4247,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="29" t="s">
         <v>72</v>
       </c>
@@ -4199,7 +4267,7 @@
         <v>180000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="31" t="s">
         <v>73</v>
       </c>
@@ -4219,47 +4287,47 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -4275,24 +4343,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
@@ -4311,24 +4383,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
@@ -4347,26 +4423,28 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4374,7 +4452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -4382,7 +4460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>72</v>
       </c>
@@ -4390,7 +4468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="4" t="s">
         <v>73</v>
       </c>
@@ -4398,34 +4476,34 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="14"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="2"/>
     </row>
   </sheetData>
@@ -4439,24 +4517,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>51</v>
       </c>
@@ -4475,33 +4557,33 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4521,7 +4603,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -4541,7 +4623,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -4561,7 +4643,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -4581,7 +4663,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -4601,7 +4683,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -4621,7 +4703,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -4653,24 +4735,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>88</v>
       </c>
@@ -4689,24 +4775,28 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
@@ -4725,23 +4815,25 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="10.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>92</v>
       </c>
@@ -4752,7 +4844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -4762,7 +4854,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -4772,7 +4864,7 @@
       <c r="C4" s="10"/>
       <c r="D4" s="33"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -4782,7 +4874,7 @@
       </c>
       <c r="D5" s="33"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
@@ -4792,7 +4884,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="4" t="s">
         <v>73</v>
       </c>
@@ -4813,24 +4905,28 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="29" t="s">
         <v>72</v>
       </c>
@@ -4838,7 +4934,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="31" t="s">
         <v>73</v>
       </c>
@@ -4856,25 +4952,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35585569-7889-4883-A327-3B12D4AB6358}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="29" t="s">
         <v>72</v>
       </c>
@@ -4882,7 +4982,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="31" t="s">
         <v>73</v>
       </c>
@@ -4901,26 +5001,26 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.28515625" style="1"/>
-    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5703125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="4.41796875" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.26171875" style="1"/>
+    <col min="15" max="15" width="12.15625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
@@ -4941,7 +5041,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4959,7 +5059,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -4977,7 +5077,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -4995,7 +5095,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -5025,33 +5125,33 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
@@ -5074,7 +5174,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -5094,7 +5194,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5114,7 +5214,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -5134,7 +5234,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -5154,7 +5254,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -5174,7 +5274,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -5206,33 +5306,33 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -5253,7 +5353,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -5273,7 +5373,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5293,7 +5393,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -5313,7 +5413,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -5333,7 +5433,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -5353,7 +5453,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -5384,33 +5484,33 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -5431,7 +5531,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -5451,7 +5551,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5471,7 +5571,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -5491,7 +5591,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -5511,7 +5611,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -5531,7 +5631,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -5562,31 +5662,31 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -5607,7 +5707,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -5627,7 +5727,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5647,7 +5747,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -5667,7 +5767,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -5687,7 +5787,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -5707,7 +5807,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>

</xml_diff>